<commit_message>
Bug fixes for production.
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\MaxLearnaqa\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadeembaig/Desktop/MaxLearnaqa-mac_version Staging/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8BA4C2-02F0-4516-9857-013418B7D499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299E1590-2342-F548-81F0-0F846A47B940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,20 +939,20 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -963,7 +963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -974,7 +974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -998,7 +998,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>9</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="E5" s="21"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>11</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1042,7 +1042,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1050,7 +1050,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>14</v>
       </c>
@@ -1064,7 +1064,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="15"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>15</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>16</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="15"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>18</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>20</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>3</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>24</v>
       </c>
@@ -1138,40 +1138,40 @@
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="24"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1199,17 +1199,17 @@
       <selection activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="6" width="36" style="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>106</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>120</v>
       </c>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>122</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>124</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1370,17 +1370,17 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -1433,12 +1433,12 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -1467,9 +1467,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -1498,18 +1498,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>39</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
@@ -1597,15 +1597,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
     </row>
@@ -1622,13 +1622,13 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>44</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>345554</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>49</v>
       </c>
@@ -1672,14 +1672,14 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>52</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>56</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>58</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
@@ -1742,19 +1742,19 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>63</v>
       </c>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -1772,14 +1772,14 @@
       </c>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>68</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>70</v>
       </c>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>72</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>74</v>
       </c>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>76</v>
       </c>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>78</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>79</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>81</v>
       </c>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>83</v>
       </c>
@@ -1860,7 +1860,7 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>85</v>
       </c>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
     </row>
@@ -1889,19 +1889,19 @@
       <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -1946,19 +1946,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -2011,19 +2011,19 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
Prod code bug fixes
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadeembaig/Desktop/MaxLearnaqa-mac_version Staging/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadeembaig/Desktop/MaxLearnaqa-mac_version/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299E1590-2342-F548-81F0-0F846A47B940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECEBADF-1933-6C4C-BF1C-D017816110B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1840" yWindow="540" windowWidth="34600" windowHeight="18800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="143">
   <si>
     <t>Admin Login</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Add category Name *</t>
   </si>
   <si>
-    <t>Accounting</t>
-  </si>
-  <si>
     <t>New Category Description *</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Subject Title *</t>
   </si>
   <si>
-    <t xml:space="preserve">Business law </t>
-  </si>
-  <si>
     <t>Subject description*</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
     <t>Designation*</t>
   </si>
   <si>
-    <t>HR Manager</t>
-  </si>
-  <si>
     <t>Country*</t>
   </si>
   <si>
@@ -437,21 +428,6 @@
     <t>Maxlearn@1</t>
   </si>
   <si>
-    <t>Anti Money Laundering New</t>
-  </si>
-  <si>
-    <t>Kyc</t>
-  </si>
-  <si>
-    <t>AML_KYC New</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>maxlearnstaging</t>
-  </si>
-  <si>
     <t>Headline</t>
   </si>
   <si>
@@ -468,25 +444,33 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Max@learn123</t>
+  </si>
+  <si>
+    <t>nadeem.baig+demoaccount@maxlearn.com</t>
+  </si>
+  <si>
+    <t>demoaccount</t>
+  </si>
+  <si>
+    <t>Financial Crimes</t>
+  </si>
+  <si>
+    <t>Anti-Bribery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -517,20 +501,6 @@
       <color rgb="FF4D5156"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF202124"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1B1B1B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -617,16 +587,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -636,30 +606,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -938,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -979,10 +947,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="7"/>
@@ -1026,8 +994,8 @@
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
+      <c r="B7" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
@@ -1069,10 +1037,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1131,8 +1099,8 @@
       <c r="A16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>139</v>
+      <c r="B16" s="31" t="s">
+        <v>140</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1196,7 +1164,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1211,105 +1179,105 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G4" s="9" t="b">
         <v>1</v>
@@ -1319,31 +1287,31 @@
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1377,44 +1345,44 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1440,18 +1408,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1471,18 +1439,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1494,7 +1462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="272" zoomScaleNormal="272" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1513,88 +1481,88 @@
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>26</v>
+      <c r="B2" s="31" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1630,7 +1598,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
@@ -1641,21 +1609,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>345554</v>
@@ -1663,10 +1631,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="7">
         <v>123456</v>
@@ -1674,53 +1642,53 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" s="7"/>
     </row>
@@ -1738,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1750,122 +1718,122 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>64</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>64</v>
       </c>
       <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C14" s="12"/>
     </row>
@@ -1886,7 +1854,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1897,40 +1865,40 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>135</v>
+        <v>88</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>136</v>
+        <v>89</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1943,7 +1911,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1954,48 +1922,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" t="s">
-        <v>138</v>
+        <v>95</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>135</v>
+        <v>88</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>136</v>
+        <v>89</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2008,7 +1976,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2019,48 +1987,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>135</v>
+        <v>88</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>136</v>
+        <v>89</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>137</v>
+        <v>102</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>